<commit_message>
Saving the cp replication data
</commit_message>
<xml_diff>
--- a/data-folder/CP replication data/Results.xlsx
+++ b/data-folder/CP replication data/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveeur-my.sharepoint.com/personal/594941jc_eur_nl/Documents/Desktop/BondRiskML/data-folder/CP replication data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_F25DC773A252ABDACC10486EC19E42C05ADE58E0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D02D8BF-AB01-4A51-B140-C196FBDABBDC}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC10486EC19E42C05ADE58E0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA071905-95D6-4A6F-82CE-536FEDCE2CD7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,7 +376,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -438,19 +438,19 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="C3">
-        <v>-2.157</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D3">
-        <v>-0.318</v>
+        <v>-1.3149999999999999</v>
       </c>
       <c r="E3">
-        <v>5.0199999999999996</v>
+        <v>-1.82</v>
       </c>
       <c r="F3">
-        <v>-2.3610000000000002</v>
+        <v>-4.2110000000000003</v>
       </c>
       <c r="G3">
-        <v>-0.06</v>
+        <v>-3.5720000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>